<commit_message>
issues related to final fixes
</commit_message>
<xml_diff>
--- a/frontend/build/users.xlsx
+++ b/frontend/build/users.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
-    <t>NAME</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
   </si>
   <si>
     <t>EMAIL</t>
@@ -28,41 +31,44 @@
     <t>Flat</t>
   </si>
   <si>
-    <t>Jasmin Mistry</t>
+    <t>Jasmin</t>
+  </si>
+  <si>
+    <t>Mistry</t>
   </si>
   <si>
     <r>
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>jasmin_13790@yahoo.co.in</t>
+      <t>jasmin_13799@yahoo.co.in</t>
     </r>
   </si>
   <si>
-    <t>Admin</t>
+    <t>tenant</t>
   </si>
   <si>
     <t>North Park Manor</t>
   </si>
   <si>
-    <t>Jasmin N</t>
+    <t>Jen</t>
+  </si>
+  <si>
+    <t>MIstry</t>
   </si>
   <si>
     <r>
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>mistry.jasmin1@gmail.com</t>
+      <t>mistry.jjasmin1@gmail.com</t>
     </r>
-  </si>
-  <si>
-    <t>Renter</t>
   </si>
   <si>
     <t>Fisgard House</t>
@@ -100,7 +106,7 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color indexed="14"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -135,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -178,40 +184,10 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -226,6 +202,66 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
@@ -254,7 +290,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -276,34 +312,43 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -328,6 +373,7 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1359,14 +1405,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1385,222 +1431,250 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
       <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" ht="40.55" customHeight="1">
       <c r="A2" t="s" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8">
-        <v>202</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9">
+        <v>402</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" ht="32.05" customHeight="1">
-      <c r="A3" t="s" s="10">
+      <c r="A3" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="12">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E3" s="13">
-        <v>202</v>
-      </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="E3" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="F3" s="15">
+        <v>402</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="jasmin_13790@yahoo.co.in"/>
-    <hyperlink ref="B3" r:id="rId2" location="" tooltip="" display="mistry.jasmin1@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="jasmin_13799@yahoo.co.in"/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="mistry.jjasmin1@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>